<commit_message>
Importacao Produto: Muda estilo status para chip padrão; Inclui novo modelo de planilha
</commit_message>
<xml_diff>
--- a/frontend/public/resources/planilha-modelo-importacao-de-produtos.xlsx
+++ b/frontend/public/resources/planilha-modelo-importacao-de-produtos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilberto.alves.ADUANEIRAS.000\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielnazari/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BCA20D-0E40-4B44-BB37-76061D17F94A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F809CC-0700-5E4B-B45D-184266AF4D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{1B6567DE-66EF-42C0-AE31-AC4E33DB4A6A}"/>
+    <workbookView xWindow="-860" yWindow="-16620" windowWidth="29400" windowHeight="16620" xr2:uid="{1B6567DE-66EF-42C0-AE31-AC4E33DB4A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo" sheetId="1" r:id="rId1"/>
@@ -25,21 +25,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Denominação</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>NCM</t>
   </si>
   <si>
-    <t>Código Interno / Partnumber</t>
-  </si>
-  <si>
-    <t>FI83902D, FI38990E, FI93882S</t>
-  </si>
-  <si>
-    <t>Fibra óptica</t>
+    <t>Código Interno</t>
+  </si>
+  <si>
+    <t>Fabricante</t>
+  </si>
+  <si>
+    <t>Operador Estrangeiro</t>
+  </si>
+  <si>
+    <t>Descricao Curta Produto</t>
+  </si>
+  <si>
+    <t>Descricao Longa Produto</t>
+  </si>
+  <si>
+    <t>03630028</t>
+  </si>
+  <si>
+    <t>01260079</t>
+  </si>
+  <si>
+    <t>03020770</t>
+  </si>
+  <si>
+    <t>85044021</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t>CONVERSOR TENSAO</t>
+  </si>
+  <si>
+    <t>CONVERSOR ESTÁTICO, RETIFICADOR, A BASE SEMICONDUTORES</t>
+  </si>
+  <si>
+    <t>AT,NS,BR</t>
+  </si>
+  <si>
+    <t>ZA,DE,SA</t>
+  </si>
+  <si>
+    <t>669790</t>
+  </si>
+  <si>
+    <t>669888</t>
+  </si>
+  <si>
+    <t>669666</t>
   </si>
 </sst>
 </file>
@@ -83,10 +122,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,52 +466,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC02B605-DF36-4C0E-BCA8-456D66B3930D}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" customWidth="1"/>
-    <col min="4" max="4" width="61.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.83203125" style="4"/>
+    <col min="6" max="6" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1"/>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>90011011</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2"/>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D3" s="2"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D4" s="2"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D9" s="1"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>